<commit_message>
Added Mongo DB Schema, basic app folder structure
Added Mongo DB Schema, basic app folder structure with login,
registration, logout and master page functionalities, Mongo db data
modelling guide
</commit_message>
<xml_diff>
--- a/2. Project Development/2. Design/TripleS_Data_Dictionary-V0.1d.xlsx
+++ b/2. Project Development/2. Design/TripleS_Data_Dictionary-V0.1d.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="142">
   <si>
     <t>Table Name</t>
   </si>
@@ -265,9 +265,6 @@
     <t>Course_Name</t>
   </si>
   <si>
-    <t>Academic_Year</t>
-  </si>
-  <si>
     <t>Percentage_Marks</t>
   </si>
   <si>
@@ -401,6 +398,51 @@
   </si>
   <si>
     <t>Student_Course_Details_ID</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>EmailID</t>
+  </si>
+  <si>
+    <t>MobileNo</t>
+  </si>
+  <si>
+    <t>CreatedDate</t>
+  </si>
+  <si>
+    <t>CreatedTime</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>DisplayUserName</t>
+  </si>
+  <si>
+    <t>RoleID</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>Composite Primary Key (UserID,RoleID)</t>
+  </si>
+  <si>
+    <t>UserID - Foreign Key(User_Master(UserID))</t>
+  </si>
+  <si>
+    <t>RoleID - Foreign Key(Role_Master(RoleID))</t>
+  </si>
+  <si>
+    <t>Passing_Year</t>
   </si>
 </sst>
 </file>
@@ -436,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -457,10 +499,13 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -756,11 +801,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -804,761 +849,771 @@
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="C3" s="1" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="2">
+      <c r="C4" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="C6" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="C8" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="C9" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="C10" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2">
+      <c r="C11" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="C12" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="7">
+      <c r="C13" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="C14" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="9">
         <v>4</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="90">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="45">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="7"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="8"/>
       <c r="C16" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="90">
+      <c r="A17" s="9"/>
       <c r="B17" s="8"/>
       <c r="C17" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="7"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="8"/>
       <c r="C18" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="7"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="8"/>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="7"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="8"/>
       <c r="C20" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="45">
-      <c r="A21" s="7"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="9"/>
       <c r="B21" s="8"/>
       <c r="C21" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>124</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="45">
-      <c r="A22" s="7"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="8"/>
       <c r="C22" s="1" t="s">
-        <v>122</v>
+        <v>44</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="30" customHeight="1">
-      <c r="A23" s="7">
-        <v>5</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>115</v>
-      </c>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="9"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" customHeight="1">
-      <c r="A24" s="7"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="9"/>
       <c r="B24" s="8"/>
       <c r="C24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" customHeight="1">
-      <c r="A25" s="7"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="9"/>
       <c r="B25" s="8"/>
       <c r="C25" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="7"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="8"/>
       <c r="C26" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="7"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="8"/>
       <c r="C27" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="30">
-      <c r="A28" s="7"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="45">
+      <c r="A28" s="9"/>
       <c r="B28" s="8"/>
       <c r="C28" s="1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="7"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="45">
+      <c r="A29" s="9"/>
       <c r="B29" s="8"/>
       <c r="C29" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="7"/>
-      <c r="B30" s="8"/>
+        <v>121</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="30" customHeight="1">
+      <c r="A30" s="9">
+        <v>5</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>114</v>
+      </c>
       <c r="C30" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30">
-      <c r="A31" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" customHeight="1">
+      <c r="A31" s="9"/>
       <c r="B31" s="8"/>
       <c r="C31" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="7"/>
+        <v>52</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30" customHeight="1">
+      <c r="A32" s="9"/>
       <c r="B32" s="8"/>
       <c r="C32" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="30">
-      <c r="A33" s="7"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="9"/>
       <c r="B33" s="8"/>
       <c r="C33" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>121</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="7"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="8"/>
       <c r="C34" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="7"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30">
+      <c r="A35" s="9"/>
       <c r="B35" s="8"/>
       <c r="C35" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="30">
-      <c r="A36" s="7"/>
+        <v>115</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="9"/>
       <c r="B36" s="8"/>
       <c r="C36" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="30">
-      <c r="A37" s="7"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="9"/>
       <c r="B37" s="8"/>
       <c r="C37" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="7"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30">
+      <c r="A38" s="9"/>
       <c r="B38" s="8"/>
       <c r="C38" s="1" t="s">
-        <v>20</v>
+        <v>116</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="7"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="8"/>
       <c r="C39" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="7">
-        <v>6</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>51</v>
-      </c>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="30">
+      <c r="A40" s="9"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="30">
-      <c r="A41" s="7"/>
+        <v>119</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="9"/>
       <c r="B41" s="8"/>
       <c r="C41" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="7"/>
+      <c r="A42" s="9"/>
       <c r="B42" s="8"/>
       <c r="C42" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="7"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="30">
+      <c r="A43" s="9"/>
       <c r="B43" s="8"/>
       <c r="C43" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="7"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="30">
+      <c r="A44" s="9"/>
       <c r="B44" s="8"/>
       <c r="C44" s="1" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="7"/>
+      <c r="A45" s="9"/>
       <c r="B45" s="8"/>
       <c r="C45" s="1" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="7"/>
+      <c r="A46" s="9"/>
       <c r="B46" s="8"/>
       <c r="C46" s="1" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="7"/>
-      <c r="B47" s="8"/>
+      <c r="A47" s="9">
+        <v>6</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="C47" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="30">
+      <c r="A48" s="9"/>
       <c r="B48" s="8"/>
       <c r="C48" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="7"/>
+      <c r="A49" s="9"/>
       <c r="B49" s="8"/>
       <c r="C49" s="1" t="s">
-        <v>59</v>
+        <v>107</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="7">
-        <v>7</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="A50" s="9"/>
+      <c r="B50" s="8"/>
       <c r="C50" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="30">
-      <c r="A51" s="7"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="9"/>
       <c r="B51" s="8"/>
       <c r="C51" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="7"/>
+      <c r="A52" s="9"/>
       <c r="B52" s="8"/>
       <c r="C52" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="7"/>
+      <c r="A53" s="9"/>
       <c r="B53" s="8"/>
       <c r="C53" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="7"/>
+      <c r="A54" s="9"/>
       <c r="B54" s="8"/>
       <c r="C54" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="7"/>
+      <c r="A55" s="9"/>
       <c r="B55" s="8"/>
       <c r="C55" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="7"/>
+      <c r="A56" s="9"/>
       <c r="B56" s="8"/>
       <c r="C56" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="7"/>
-      <c r="B57" s="8"/>
+      <c r="A57" s="9">
+        <v>7</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="C57" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="30">
+      <c r="A58" s="9"/>
       <c r="B58" s="8"/>
       <c r="C58" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="7">
-        <v>8</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>107</v>
-      </c>
+      <c r="A59" s="9"/>
+      <c r="B59" s="8"/>
       <c r="C59" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="30">
-      <c r="A60" s="7"/>
+        <v>67</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="9"/>
       <c r="B60" s="8"/>
       <c r="C60" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="7"/>
+      <c r="A61" s="9"/>
       <c r="B61" s="8"/>
       <c r="C61" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="30">
-      <c r="A62" s="7"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="9"/>
       <c r="B62" s="8"/>
       <c r="C62" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="7"/>
+      <c r="A63" s="9"/>
       <c r="B63" s="8"/>
       <c r="C63" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="7"/>
+      <c r="A64" s="9"/>
       <c r="B64" s="8"/>
       <c r="C64" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="7"/>
+      <c r="A65" s="9"/>
       <c r="B65" s="8"/>
       <c r="C65" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:7">
-      <c r="A66" s="7"/>
-      <c r="B66" s="8"/>
+      <c r="A66" s="9">
+        <v>8</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>106</v>
+      </c>
       <c r="C66" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="30">
+      <c r="A67" s="9"/>
       <c r="B67" s="8"/>
       <c r="C67" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>79</v>
+        <v>52</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="7"/>
+      <c r="A68" s="9"/>
       <c r="B68" s="8"/>
       <c r="C68" s="1" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="7"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="30">
+      <c r="A69" s="9"/>
       <c r="B69" s="8"/>
       <c r="C69" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="7"/>
+      <c r="A70" s="9"/>
       <c r="B70" s="8"/>
       <c r="C70" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="7"/>
+      <c r="A71" s="9"/>
       <c r="B71" s="8"/>
       <c r="C71" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="7"/>
+      <c r="A72" s="9"/>
       <c r="B72" s="8"/>
       <c r="C72" s="1" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="7"/>
+      <c r="A73" s="9"/>
       <c r="B73" s="8"/>
       <c r="C73" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="7"/>
+      <c r="A74" s="9"/>
       <c r="B74" s="8"/>
       <c r="C74" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="7"/>
+      <c r="A75" s="9"/>
       <c r="B75" s="8"/>
       <c r="C75" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76" s="7"/>
+      <c r="A76" s="9"/>
       <c r="B76" s="8"/>
       <c r="C76" s="1" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:7">
-      <c r="A77" s="7"/>
+      <c r="A77" s="9"/>
       <c r="B77" s="8"/>
       <c r="C77" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="30">
-      <c r="A78" s="4">
+    <row r="78" spans="1:7">
+      <c r="A78" s="9"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="9"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="9"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="9"/>
+      <c r="B81" s="8"/>
+      <c r="C81" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="9"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="9"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" s="9"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="30">
+      <c r="A85" s="4">
         <v>9</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B85" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="30">
+      <c r="A86" s="6"/>
+      <c r="B86" s="5"/>
+      <c r="C86" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" s="4"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="4"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="30">
-      <c r="A79" s="6"/>
-      <c r="B79" s="5"/>
-      <c r="C79" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80" s="4"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7">
-      <c r="A81" s="4"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="1" t="s">
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" s="4"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
-      <c r="A82" s="4"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="1" t="s">
+    <row r="90" spans="1:7">
+      <c r="A90" s="4"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
-      <c r="A83" s="4"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="30" customHeight="1">
-      <c r="A84" s="7">
+    <row r="91" spans="1:7" ht="30" customHeight="1">
+      <c r="A91" s="9">
         <v>10</v>
       </c>
-      <c r="B84" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="30">
-      <c r="A85" s="7"/>
-      <c r="B85" s="8"/>
-      <c r="C85" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="45">
-      <c r="A86" s="7"/>
-      <c r="B86" s="8"/>
-      <c r="C86" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="30">
-      <c r="A87" s="7"/>
-      <c r="B87" s="8"/>
-      <c r="C87" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
-      <c r="A88" s="7"/>
-      <c r="B88" s="8"/>
-      <c r="C88" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="A89" s="7"/>
-      <c r="B89" s="8"/>
-      <c r="C89" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7">
-      <c r="A90" s="7"/>
-      <c r="B90" s="8"/>
-      <c r="C90" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7">
-      <c r="A91" s="7">
-        <v>11</v>
-      </c>
       <c r="B91" s="8" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>11</v>
@@ -1567,199 +1622,265 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
-      <c r="A92" s="7"/>
+    <row r="92" spans="1:7" ht="30">
+      <c r="A92" s="9"/>
       <c r="B92" s="8"/>
       <c r="C92" s="1" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7">
-      <c r="A93" s="7"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="45">
+      <c r="A93" s="9"/>
       <c r="B93" s="8"/>
-      <c r="C93" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>89</v>
+      <c r="C93" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="30">
-      <c r="A94" s="7"/>
+      <c r="A94" s="9"/>
       <c r="B94" s="8"/>
       <c r="C94" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="30">
-      <c r="A95" s="7"/>
+        <v>77</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" s="9"/>
       <c r="B95" s="8"/>
       <c r="C95" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
     </row>
     <row r="96" spans="1:7">
-      <c r="A96" s="7"/>
+      <c r="A96" s="9"/>
       <c r="B96" s="8"/>
       <c r="C96" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="97" spans="1:7">
-      <c r="A97" s="7"/>
+      <c r="A97" s="9"/>
       <c r="B97" s="8"/>
       <c r="C97" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:7">
-      <c r="A98" s="7"/>
-      <c r="B98" s="8"/>
+      <c r="A98" s="9">
+        <v>11</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="C98" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>97</v>
+        <v>11</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:7">
-      <c r="A99" s="7">
-        <v>12</v>
-      </c>
-      <c r="B99" s="8" t="s">
-        <v>99</v>
-      </c>
+      <c r="A99" s="9"/>
+      <c r="B99" s="8"/>
       <c r="C99" s="1" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>12</v>
+        <v>87</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="100" spans="1:7">
-      <c r="A100" s="7"/>
+      <c r="A100" s="9"/>
       <c r="B100" s="8"/>
       <c r="C100" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F100" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G100" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G100" s="1" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="101" spans="1:7" ht="30">
-      <c r="A101" s="7"/>
+      <c r="A101" s="9"/>
       <c r="B101" s="8"/>
       <c r="C101" s="1" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="45">
-      <c r="A102" s="7"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="30">
+      <c r="A102" s="9"/>
       <c r="B102" s="8"/>
       <c r="C102" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>106</v>
+        <v>91</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="103" spans="1:7">
-      <c r="A103" s="7"/>
+      <c r="A103" s="9"/>
       <c r="B103" s="8"/>
       <c r="C103" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="30">
-      <c r="A104" s="7"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" s="9"/>
       <c r="B104" s="8"/>
       <c r="C104" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="105" spans="1:7">
-      <c r="A105" s="7"/>
+      <c r="A105" s="9"/>
       <c r="B105" s="8"/>
       <c r="C105" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="106" spans="1:7">
-      <c r="A106" s="7"/>
-      <c r="B106" s="8"/>
+      <c r="A106" s="9">
+        <v>12</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>98</v>
+      </c>
       <c r="C106" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G106" s="1" t="s">
-        <v>98</v>
+        <v>11</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:7">
-      <c r="A107" s="7"/>
+      <c r="A107" s="9"/>
       <c r="B107" s="8"/>
       <c r="C107" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="30">
+      <c r="A108" s="9"/>
+      <c r="B108" s="8"/>
+      <c r="C108" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="45">
+      <c r="A109" s="9"/>
+      <c r="B109" s="8"/>
+      <c r="C109" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" s="9"/>
+      <c r="B110" s="8"/>
+      <c r="C110" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="30">
+      <c r="A111" s="9"/>
+      <c r="B111" s="8"/>
+      <c r="C111" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G111" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G107" s="1" t="s">
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" s="9"/>
+      <c r="B112" s="8"/>
+      <c r="C112" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" s="9"/>
+      <c r="B113" s="8"/>
+      <c r="C113" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G113" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
-      <c r="A108" s="2">
+    <row r="114" spans="1:7">
+      <c r="A114" s="9"/>
+      <c r="B114" s="8"/>
+      <c r="C114" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" s="2">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="B91:B98"/>
-    <mergeCell ref="A91:A98"/>
-    <mergeCell ref="B99:B107"/>
-    <mergeCell ref="A99:A107"/>
-    <mergeCell ref="B59:B77"/>
-    <mergeCell ref="A59:A77"/>
-    <mergeCell ref="A84:A90"/>
-    <mergeCell ref="B84:B90"/>
-    <mergeCell ref="B40:B49"/>
-    <mergeCell ref="A40:A49"/>
-    <mergeCell ref="B50:B58"/>
-    <mergeCell ref="A50:A58"/>
-    <mergeCell ref="B8:B22"/>
-    <mergeCell ref="A8:A22"/>
-    <mergeCell ref="A23:A39"/>
-    <mergeCell ref="B23:B39"/>
+  <mergeCells count="17">
+    <mergeCell ref="B98:B105"/>
+    <mergeCell ref="A98:A105"/>
+    <mergeCell ref="B106:B114"/>
+    <mergeCell ref="A106:A114"/>
+    <mergeCell ref="B66:B84"/>
+    <mergeCell ref="A66:A84"/>
+    <mergeCell ref="A91:A97"/>
+    <mergeCell ref="B91:B97"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B47:B56"/>
+    <mergeCell ref="A47:A56"/>
+    <mergeCell ref="B57:B65"/>
+    <mergeCell ref="A57:A65"/>
+    <mergeCell ref="B15:B29"/>
+    <mergeCell ref="A15:A29"/>
+    <mergeCell ref="A30:A46"/>
+    <mergeCell ref="B30:B46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>